<commit_message>
Update test results for Raspberry Pi
Added test result for Pi 4B 32-bit Raspbian.
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
   <si>
     <t>CentOS</t>
   </si>
@@ -39,15 +39,6 @@
     <t>x86_64</t>
   </si>
   <si>
-    <t>Distro</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>Architecture</t>
-  </si>
-  <si>
     <t>Ubuntu</t>
   </si>
   <si>
@@ -57,9 +48,6 @@
     <t>Mint</t>
   </si>
   <si>
-    <t>Host</t>
-  </si>
-  <si>
     <t>VMware</t>
   </si>
   <si>
@@ -156,13 +144,40 @@
     <t>gcc 7.4.0</t>
   </si>
   <si>
-    <t>Real Hardware</t>
-  </si>
-  <si>
     <t>9.0</t>
   </si>
   <si>
     <t>not ready yet</t>
+  </si>
+  <si>
+    <t>Raspbian</t>
+  </si>
+  <si>
+    <t>armv7l</t>
+  </si>
+  <si>
+    <t>VMware indicates VMware 15.5 running on Windows 10 running on Intel i7 CPU</t>
+  </si>
+  <si>
+    <t>Target OS</t>
+  </si>
+  <si>
+    <t>AMD64 Server</t>
+  </si>
+  <si>
+    <t>OS Version</t>
+  </si>
+  <si>
+    <t>Target CPU Architecture</t>
+  </si>
+  <si>
+    <t>All builds are compiled natively on the target OS (not cross compiled)</t>
+  </si>
+  <si>
+    <t>All builds match the bitness of the installed OS</t>
+  </si>
+  <si>
+    <t>System Hardware</t>
   </si>
 </sst>
 </file>
@@ -218,7 +233,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -240,6 +255,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -536,16 +554,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G31"/>
+  <dimension ref="A2:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
@@ -555,7 +573,7 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -565,124 +583,73 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44178</v>
+        <v>44179</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="B6" s="2"/>
-      <c r="F6" s="4"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>41</v>
+      <c r="A7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="6">
-        <v>44177</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="6">
-        <v>44177</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="6">
-        <v>44177</v>
+      <c r="B10" s="2"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="30.75" customHeight="1">
+      <c r="A11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5">
-        <v>10.6</v>
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F12" s="6">
         <v>44177</v>
@@ -690,185 +657,179 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="5">
-        <v>9.9</v>
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F13" s="6">
         <v>44177</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="5">
-        <v>8.6</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="6">
-        <v>44177</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="5">
-        <v>8.6</v>
+      <c r="B15" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="6">
+        <v>44177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="5">
+        <v>10.6</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="6">
-        <v>44177</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="9"/>
+      <c r="D16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="6">
+        <v>44179</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B17" s="5">
-        <v>20.04</v>
+        <v>9.9</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17" s="6">
-        <v>44178</v>
+        <v>44177</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B18" s="5">
-        <v>18.04</v>
+        <v>8.6</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F18" s="6">
         <v>44177</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B19" s="5">
-        <v>12.04</v>
+        <v>8.6</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F19" s="6">
         <v>44177</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="5">
-        <v>12.04</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="6">
-        <v>44177</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="5"/>
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5">
+        <v>20.04</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="6">
+        <v>44178</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B22" s="5">
-        <v>11.19</v>
+        <v>18.04</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F22" s="6">
         <v>44177</v>
@@ -876,132 +837,227 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B23" s="5">
-        <v>20.04</v>
+        <v>12.04</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="6">
+        <v>44177</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="6">
-        <v>44177</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B24" s="5">
-        <v>20</v>
+        <v>12.04</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="6">
+        <v>44177</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="6">
-        <v>44178</v>
-      </c>
     </row>
     <row r="25" spans="1:7">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B26" s="5">
-        <v>15.1</v>
+        <v>11.19</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>42</v>
+        <v>10</v>
+      </c>
+      <c r="F26" s="6">
+        <v>44177</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="5">
+        <v>20.04</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="6">
+        <v>44177</v>
+      </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="B28" s="5">
+        <v>20</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F28" s="6">
         <v>44178</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="5" t="s">
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="5">
+        <v>15.1</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="6">
+        <v>44178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29" s="6">
-        <v>44177</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
+      <c r="C33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="6">
+        <v>44177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="6">
+        <v>43978</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="6">
+        <v>44178</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test results matrix
Update test results for Pi.
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -560,7 +560,7 @@
   <dimension ref="A2:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -586,7 +586,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44185</v>
+        <v>44187</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -721,7 +721,7 @@
         <v>10</v>
       </c>
       <c r="F16" s="6">
-        <v>44179</v>
+        <v>44187</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1124,7 +1124,7 @@
         <v>18</v>
       </c>
       <c r="F38" s="6">
-        <v>44177</v>
+        <v>44187</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1144,7 +1144,7 @@
         <v>16</v>
       </c>
       <c r="F39" s="6">
-        <v>44178</v>
+        <v>44187</v>
       </c>
       <c r="G39" s="9" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Fix for CentOS Stream 8
Fix detection for CentOS Stream 8.
Fix name of CMAKE package on CentOS 8.
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="64">
   <si>
     <t>CentOS</t>
   </si>
@@ -193,6 +193,21 @@
   </si>
   <si>
     <t>openSUSE</t>
+  </si>
+  <si>
+    <t>RAM Size</t>
+  </si>
+  <si>
+    <t>2 GB</t>
+  </si>
+  <si>
+    <t>4 GB</t>
+  </si>
+  <si>
+    <t>Stream 8</t>
+  </si>
+  <si>
+    <t>gcc 8.4.1</t>
   </si>
 </sst>
 </file>
@@ -572,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G43"/>
+  <dimension ref="A2:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -583,54 +598,56 @@
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44203</v>
+        <v>44210</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="B10" s="2"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" ht="30.75" customHeight="1">
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="30.75" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>45</v>
       </c>
@@ -640,147 +657,158 @@
       <c r="C11" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="6">
-        <v>44203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>63</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6">
+        <v>44210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="6">
+        <v>44210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="6">
-        <v>44203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="6">
-        <v>44203</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="F14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="6">
+        <v>44210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="5">
-        <v>10.6</v>
+      <c r="B16" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="6">
-        <v>44187</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="F16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="6">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="5">
-        <v>9.9</v>
+        <v>10.6</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="6">
-        <v>44177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>25</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="6">
+        <v>44187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="5">
-        <v>8.6</v>
+        <v>9.9</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="6">
-        <v>44183</v>
-      </c>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="1:7">
+        <v>26</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="6">
+        <v>44177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -790,18 +818,19 @@
       <c r="C19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="6">
-        <v>44182</v>
-      </c>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="1:7">
+        <v>25</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="6">
+        <v>44183</v>
+      </c>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -811,20 +840,19 @@
       <c r="C20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="6">
-        <v>44185</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>26</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="6">
+        <v>44182</v>
+      </c>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -834,20 +862,21 @@
       <c r="C21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="6">
-        <v>44177</v>
-      </c>
-      <c r="G21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="6">
+        <v>44185</v>
+      </c>
+      <c r="H21" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -857,51 +886,56 @@
       <c r="C22" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="6">
+        <v>44177</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5">
+        <v>8.6</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="6">
+      <c r="F23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="6">
         <v>44177</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="H23" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
+    <row r="24" spans="1:8">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
         <v>57</v>
-      </c>
-      <c r="B24" s="5">
-        <v>20.04</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" s="6">
-        <v>44203</v>
-      </c>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>7</v>
       </c>
       <c r="B25" s="5">
         <v>20.04</v>
@@ -909,58 +943,61 @@
       <c r="C25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="5"/>
+      <c r="E25" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="6">
-        <v>44178</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="F25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="6">
+        <v>44203</v>
+      </c>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="5">
-        <v>18.04</v>
+        <v>20.04</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="6">
-        <v>44177</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>30</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="6">
+        <v>44178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="5">
-        <v>12.04</v>
+        <v>18.04</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D27" s="5"/>
       <c r="E27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="6">
-        <v>44183</v>
-      </c>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="1:7">
+        <v>28</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="6">
+        <v>44177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -970,18 +1007,19 @@
       <c r="C28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="6">
-        <v>44182</v>
-      </c>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="1:7">
+        <v>25</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="6">
+        <v>44183</v>
+      </c>
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -991,20 +1029,19 @@
       <c r="C29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="6">
-        <v>44177</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>26</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="6">
+        <v>44182</v>
+      </c>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1014,214 +1051,252 @@
       <c r="C30" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="6">
+        <v>44177</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="5">
+        <v>12.04</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="6">
+      <c r="F31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="6">
         <v>44177</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="H31" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="5">
-        <v>11.19</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="6">
-        <v>44177</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+    <row r="32" spans="1:8">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>12</v>
       </c>
       <c r="B33" s="5">
-        <v>20.04</v>
+        <v>11.19</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="D33" s="5"/>
       <c r="E33" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="6">
+        <v>28</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G33" s="6">
         <v>44177</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B34" s="5">
-        <v>20</v>
+        <v>20.04</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="6">
+      <c r="F34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G34" s="6">
+        <v>44205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="5">
+        <v>20</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="6">
         <v>44178</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
+    <row r="36" spans="1:8">
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B37" s="5">
         <v>15.1</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C37" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D37" s="5"/>
+      <c r="E37" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="6">
+      <c r="F37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" s="6">
         <v>44203</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" t="s">
+    <row r="38" spans="1:8">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F38" s="6">
-        <v>44178</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" s="6">
+        <v>44178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="F40" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="6">
+      <c r="G40" s="6">
         <v>44203</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
-      <c r="A40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F40" s="6">
-        <v>44187</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="6">
+        <v>44187</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D42" s="5"/>
+      <c r="E42" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="F42" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F41" s="6"/>
-      <c r="G41" s="9"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" t="s">
+      <c r="G42" s="6"/>
+      <c r="H42" s="9"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B44" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D44" s="5"/>
+      <c r="E44" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="F44" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="G44" s="5" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add support for Arch/Manjaro 20
Added support for Manjaro.
Tested on Manjaro 20.2 x86_64 on VMware and 20.12 on a Pi 4B.
Arch should "just work" but I didn't test that.
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="65">
   <si>
     <t>CentOS</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>gcc 8.4.1</t>
+  </si>
+  <si>
+    <t>Manjaro</t>
   </si>
 </sst>
 </file>
@@ -587,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H44"/>
+  <dimension ref="A2:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -617,7 +620,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44210</v>
+        <v>44215</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1186,117 +1189,159 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="5">
+        <v>20.2</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="6">
+        <v>44215</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G39" s="6">
-        <v>44178</v>
-      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G40" s="6">
-        <v>44203</v>
+        <v>44178</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>56</v>
+        <v>16</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G41" s="6">
-        <v>44187</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>34</v>
+        <v>44203</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>55</v>
+      <c r="B42" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F42" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="6">
+        <v>44187</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G42" s="6"/>
-      <c r="H42" s="9"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>40</v>
+        <v>64</v>
+      </c>
+      <c r="B44" s="5">
+        <v>20.12</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" s="6">
+        <v>44215</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F46" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G44" s="5" t="s">
+      <c r="G46" s="5" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Windows to the test results.
Add Windows to the test results.
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="74">
   <si>
     <t>CentOS</t>
   </si>
@@ -126,9 +126,6 @@
     <t>gcc 4.9.3</t>
   </si>
   <si>
-    <t>Problems</t>
-  </si>
-  <si>
     <t>NetBSD</t>
   </si>
   <si>
@@ -211,6 +208,36 @@
   </si>
   <si>
     <t>Manjaro</t>
+  </si>
+  <si>
+    <t>Docker on WSL2</t>
+  </si>
+  <si>
+    <t>Docker</t>
+  </si>
+  <si>
+    <t>5.20.5</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Notes / Problems</t>
+  </si>
+  <si>
+    <t>Windows 10</t>
+  </si>
+  <si>
+    <t>Pro 20H2</t>
+  </si>
+  <si>
+    <t>6 GB</t>
+  </si>
+  <si>
+    <t>VS2017/2019</t>
+  </si>
+  <si>
+    <t>Vmware</t>
   </si>
 </sst>
 </file>
@@ -590,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H46"/>
+  <dimension ref="A2:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -602,7 +629,7 @@
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
@@ -620,7 +647,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44215</v>
+        <v>44252</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -633,17 +660,17 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -652,176 +679,150 @@
     </row>
     <row r="11" spans="1:8" ht="30.75" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>48</v>
-      </c>
       <c r="D11" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>32</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>3</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="6">
-        <v>44210</v>
-      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="E13" s="5" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="G13" s="6">
+        <v>44252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="6">
         <v>44210</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="6">
-        <v>44210</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>61</v>
-      </c>
+      <c r="D16" s="5"/>
       <c r="E16" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G16" s="6">
-        <v>44203</v>
+        <v>44210</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="5">
-        <v>10.6</v>
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="6">
-        <v>44187</v>
+        <v>44210</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="5">
-        <v>9.9</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="6">
-        <v>44177</v>
-      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="5">
-        <v>8.6</v>
+      <c r="B19" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="E19" s="5" t="s">
         <v>25</v>
       </c>
@@ -829,54 +830,49 @@
         <v>10</v>
       </c>
       <c r="G19" s="6">
-        <v>44183</v>
-      </c>
-      <c r="H19" s="9"/>
+        <v>44203</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="5">
-        <v>8.6</v>
+        <v>10.6</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="6">
-        <v>44182</v>
-      </c>
-      <c r="H20" s="9"/>
+        <v>44187</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="5">
-        <v>8.6</v>
+        <v>9.9</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="6">
-        <v>44185</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>34</v>
+        <v>44177</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -891,17 +887,15 @@
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="6">
-        <v>44177</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>34</v>
-      </c>
+        <v>44183</v>
+      </c>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
@@ -915,110 +909,116 @@
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G23" s="6">
-        <v>44177</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>33</v>
-      </c>
+        <v>44182</v>
+      </c>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5">
+        <v>8.6</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="9"/>
+      <c r="E24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="6">
+        <v>44185</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="B25" s="5">
-        <v>20.04</v>
+        <v>8.6</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G25" s="6">
-        <v>44203</v>
-      </c>
-      <c r="H25" s="9"/>
+        <v>44177</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B26" s="5">
-        <v>20.04</v>
+        <v>8.6</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G26" s="6">
-        <v>44178</v>
+        <v>44177</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="5">
-        <v>18.04</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="6">
-        <v>44177</v>
-      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B28" s="5">
-        <v>12.04</v>
+        <v>20.04</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G28" s="6">
-        <v>44183</v>
+        <v>44203</v>
       </c>
       <c r="H28" s="9"/>
     </row>
@@ -1027,45 +1027,41 @@
         <v>7</v>
       </c>
       <c r="B29" s="5">
-        <v>12.04</v>
+        <v>20.04</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G29" s="6">
-        <v>44182</v>
-      </c>
-      <c r="H29" s="9"/>
+        <v>44178</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="5">
-        <v>12.04</v>
+        <v>18.04</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G30" s="6">
         <v>44177</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1073,276 +1069,387 @@
         <v>7</v>
       </c>
       <c r="B31" s="5">
-        <v>12.04</v>
+        <v>16.04</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="G31" s="6">
-        <v>44177</v>
+        <v>44245</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="5"/>
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="5">
+        <v>12.04</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="6">
+        <v>44183</v>
+      </c>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B33" s="5">
-        <v>11.19</v>
+        <v>12.04</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G33" s="6">
-        <v>44177</v>
-      </c>
+        <v>44182</v>
+      </c>
+      <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B34" s="5">
-        <v>20.04</v>
+        <v>12.04</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>60</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G34" s="6">
-        <v>44205</v>
+        <v>44177</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B35" s="5">
-        <v>20</v>
+        <v>12.04</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G35" s="6">
-        <v>44178</v>
+        <v>44177</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:8">
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
       <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="5">
-        <v>15.1</v>
+        <v>12</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="5"/>
-      <c r="E37" s="5" t="s">
-        <v>28</v>
-      </c>
+      <c r="E37" s="5"/>
       <c r="F37" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G37" s="6">
-        <v>44203</v>
+      <c r="G37" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="B38" s="5">
-        <v>20.2</v>
+        <v>20.04</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="5"/>
+      <c r="D38" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E38" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G38" s="6">
-        <v>44215</v>
+        <v>44205</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="5">
+        <v>11.19</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="6">
+        <v>44177</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="B40" s="5">
+        <v>20</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G40" s="6">
         <v>44178</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G41" s="6">
-        <v>44203</v>
-      </c>
+      <c r="G41" s="5"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="B42" s="5">
+        <v>15.1</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G42" s="6">
-        <v>44187</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>34</v>
+        <v>44203</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>55</v>
+        <v>63</v>
+      </c>
+      <c r="B43" s="5">
+        <v>20.2</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G43" s="6">
+        <v>44215</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G43" s="6"/>
-      <c r="H43" s="9"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" t="s">
-        <v>64</v>
-      </c>
-      <c r="B44" s="5">
-        <v>20.12</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G44" s="6">
-        <v>44215</v>
+      <c r="F45" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G45" s="6">
+        <v>44178</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" s="6">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G47" s="6">
+        <v>44187</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G48" s="6"/>
+      <c r="H48" s="9"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="5">
+        <v>20.12</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49" s="6">
+        <v>44215</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F46" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>41</v>
+      <c r="C51" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test matrix for FreeBSD
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="82">
   <si>
     <t>CentOS</t>
   </si>
@@ -132,9 +132,6 @@
     <t>amd64</t>
   </si>
   <si>
-    <t>gcc 7.4.0</t>
-  </si>
-  <si>
     <t>9.0</t>
   </si>
   <si>
@@ -238,6 +235,33 @@
   </si>
   <si>
     <t>Vmware</t>
+  </si>
+  <si>
+    <t>Freebsd</t>
+  </si>
+  <si>
+    <t>arm64</t>
+  </si>
+  <si>
+    <t>Clang 10</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 3B+</t>
+  </si>
+  <si>
+    <t>'mainsize' test is skipped</t>
+  </si>
+  <si>
+    <t>13.0 RC5</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 4B</t>
+  </si>
+  <si>
+    <t>Clang 11</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
@@ -293,7 +317,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -321,6 +345,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -617,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H51"/>
+  <dimension ref="A2:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -647,7 +674,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44252</v>
+        <v>44298</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -660,17 +687,17 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -679,28 +706,28 @@
     </row>
     <row r="11" spans="1:8" ht="30.75" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="D11" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>32</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>3</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -712,22 +739,22 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
         <v>69</v>
-      </c>
-      <c r="B13" t="s">
-        <v>70</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="G13" s="6">
         <v>44252</v>
@@ -745,14 +772,14 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>10</v>
@@ -821,7 +848,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>25</v>
@@ -931,7 +958,7 @@
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>10</v>
@@ -1002,7 +1029,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" s="5">
         <v>20.04</v>
@@ -1076,16 +1103,16 @@
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G31" s="6">
         <v>44245</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1192,7 +1219,7 @@
         <v>12</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>6</v>
@@ -1203,7 +1230,7 @@
         <v>10</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1217,7 +1244,7 @@
         <v>6</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>30</v>
@@ -1276,7 +1303,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" s="5">
         <v>15.1</v>
@@ -1297,7 +1324,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B43" s="5">
         <v>20.2</v>
@@ -1368,13 +1395,13 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="s">
@@ -1392,27 +1419,27 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G48" s="6"/>
       <c r="H48" s="9"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B49" s="5">
         <v>20.12</v>
@@ -1431,25 +1458,90 @@
         <v>44215</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51" s="8">
+        <v>12.2</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G51" s="6">
+        <v>44294</v>
+      </c>
+      <c r="H51" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52" s="8">
+        <v>12.2</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G52" s="6">
+        <v>44294</v>
+      </c>
+      <c r="H52" s="12"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G53" s="6">
+        <v>44298</v>
+      </c>
+      <c r="H53" s="12"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B54" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G54" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Test Matrix for Manjaro
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -647,7 +647,7 @@
   <dimension ref="A2:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -674,7 +674,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44298</v>
+        <v>44299</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1340,7 +1340,7 @@
         <v>10</v>
       </c>
       <c r="G43" s="6">
-        <v>44215</v>
+        <v>44299</v>
       </c>
     </row>
     <row r="44" spans="1:8">

</xml_diff>

<commit_message>
Add 'libtool' to packages for MacOS
Display search path with system info.
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -315,10 +315,10 @@
     <t>Zorin</t>
   </si>
   <si>
-    <t>Zorin 15.3 is based on Ubuntu 18.04</t>
-  </si>
-  <si>
     <t>11.15.1</t>
+  </si>
+  <si>
+    <t>Zorin 15.3 seems to be based on Ubuntu 18.04</t>
   </si>
 </sst>
 </file>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -734,7 +734,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44409</v>
+        <v>44411</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1157,7 +1157,7 @@
         <v>44378</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1178,7 +1178,7 @@
         <v>9</v>
       </c>
       <c r="G31" s="6">
-        <v>44203</v>
+        <v>44411</v>
       </c>
       <c r="H31" s="9"/>
     </row>
@@ -1830,7 +1830,7 @@
         <v>78</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
For Debian, replaced 'libtool' with 'libltdl-dev'
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="109">
   <si>
     <t>CentOS</t>
   </si>
@@ -57,15 +57,9 @@
     <t>(beta)</t>
   </si>
   <si>
-    <t>Raspberry Pi 4B 8GB</t>
-  </si>
-  <si>
     <t>Ubuntu Mate</t>
   </si>
   <si>
-    <t>Raspberry Pi 4B 4GB</t>
-  </si>
-  <si>
     <t>AArch64</t>
   </si>
   <si>
@@ -165,9 +159,6 @@
     <t>gcc 5.4.0</t>
   </si>
   <si>
-    <t>Raspberry Pi Zero W</t>
-  </si>
-  <si>
     <t>armv6l</t>
   </si>
   <si>
@@ -234,18 +225,12 @@
     <t>Clang 10</t>
   </si>
   <si>
-    <t>Raspberry Pi 3B+</t>
-  </si>
-  <si>
     <t>'mainsize' test is skipped</t>
   </si>
   <si>
     <t>13.0 RC5</t>
   </si>
   <si>
-    <t>Raspberry Pi 4B</t>
-  </si>
-  <si>
     <t>Clang 11</t>
   </si>
   <si>
@@ -318,13 +303,55 @@
     <t>11.15.1</t>
   </si>
   <si>
-    <t>Zorin 15.3 seems to be based on Ubuntu 18.04</t>
+    <t>seems to be based on Ubuntu 18.04</t>
+  </si>
+  <si>
+    <t>Big Sur (Homebrew)</t>
+  </si>
+  <si>
+    <t>Big Sur (MacPorts)</t>
+  </si>
+  <si>
+    <t>Pi 4B 8GB</t>
+  </si>
+  <si>
+    <t>Pi Zero W</t>
+  </si>
+  <si>
+    <t>Pi 4B 4GB</t>
+  </si>
+  <si>
+    <t>Pi 3B+</t>
+  </si>
+  <si>
+    <t>Pi 4B</t>
+  </si>
+  <si>
+    <t>Clang 13</t>
+  </si>
+  <si>
+    <t>Monterey (Beta)</t>
+  </si>
+  <si>
+    <t>under construction</t>
+  </si>
+  <si>
+    <t>Arch</t>
+  </si>
+  <si>
+    <t>5.14.12</t>
+  </si>
+  <si>
+    <t>gcc 11.1.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -374,7 +401,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -408,6 +435,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -704,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H67"/>
+  <dimension ref="A2:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -716,15 +746,14 @@
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="5" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
     <col min="8" max="8" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -734,7 +763,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44411</v>
+        <v>44483</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -742,22 +771,22 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -766,28 +795,28 @@
     </row>
     <row r="11" spans="1:8" ht="30.75" customHeight="1">
       <c r="A11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="C11" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>47</v>
+        <v>28</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>3</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -799,24 +828,24 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G13" s="6">
+      <c r="G13" s="14">
         <v>44252</v>
       </c>
     </row>
@@ -826,11 +855,11 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B15" s="5">
         <v>8.4</v>
@@ -839,15 +868,15 @@
         <v>5</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="14">
         <v>44393</v>
       </c>
     </row>
@@ -856,19 +885,19 @@
         <v>0</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="14">
         <v>44210</v>
       </c>
     </row>
@@ -884,12 +913,12 @@
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="14">
         <v>44210</v>
       </c>
     </row>
@@ -898,25 +927,25 @@
         <v>0</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="14">
         <v>44210</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B19" s="5">
         <v>34</v>
@@ -925,15 +954,15 @@
         <v>5</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="14">
         <v>44378</v>
       </c>
     </row>
@@ -942,28 +971,28 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="G20" s="14"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="14">
         <v>44377</v>
       </c>
     </row>
@@ -975,16 +1004,16 @@
         <v>10.6</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="14">
         <v>44187</v>
       </c>
     </row>
@@ -996,16 +1025,16 @@
         <v>9.9</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="14">
         <v>44177</v>
       </c>
     </row>
@@ -1017,16 +1046,16 @@
         <v>8.6</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="14">
         <v>44183</v>
       </c>
       <c r="H24" s="9"/>
@@ -1039,16 +1068,16 @@
         <v>8.6</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="14">
         <v>44182</v>
       </c>
       <c r="H25" s="9"/>
@@ -1061,20 +1090,20 @@
         <v>8.6</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="14">
         <v>44185</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1085,20 +1114,20 @@
         <v>8.6</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="14">
         <v>44177</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1109,20 +1138,20 @@
         <v>8.6</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="14">
         <v>44177</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1131,12 +1160,12 @@
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="6"/>
+      <c r="G29" s="14"/>
       <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B30" s="5">
         <v>15.3</v>
@@ -1145,24 +1174,24 @@
         <v>5</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="14">
         <v>44378</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B31" s="5">
         <v>20.04</v>
@@ -1172,12 +1201,12 @@
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31" s="14">
         <v>44411</v>
       </c>
       <c r="H31" s="9"/>
@@ -1194,12 +1223,12 @@
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="14">
         <v>44178</v>
       </c>
     </row>
@@ -1215,12 +1244,12 @@
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="14">
         <v>44177</v>
       </c>
     </row>
@@ -1236,16 +1265,16 @@
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G34" s="6">
+        <v>59</v>
+      </c>
+      <c r="G34" s="14">
         <v>44245</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1256,16 +1285,16 @@
         <v>12.04</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35" s="14">
         <v>44183</v>
       </c>
       <c r="H35" s="9"/>
@@ -1278,16 +1307,16 @@
         <v>12.04</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G36" s="14">
         <v>44182</v>
       </c>
       <c r="H36" s="9"/>
@@ -1300,20 +1329,20 @@
         <v>12.04</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G37" s="6">
+      <c r="G37" s="14">
         <v>44177</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1324,20 +1353,20 @@
         <v>12.04</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="14">
         <v>44177</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1345,7 +1374,7 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="5"/>
+      <c r="G39" s="14"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
@@ -1358,15 +1387,15 @@
         <v>5</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40" s="14">
         <v>44383</v>
       </c>
     </row>
@@ -1381,15 +1410,15 @@
         <v>5</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="6">
+      <c r="G41" s="14">
         <v>44205</v>
       </c>
     </row>
@@ -1405,12 +1434,12 @@
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="6">
+      <c r="G42" s="14">
         <v>44177</v>
       </c>
     </row>
@@ -1426,453 +1455,531 @@
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43" s="14">
         <v>44178</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>97</v>
-      </c>
-      <c r="B44" s="5">
+        <v>106</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="14">
+        <v>44483</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="5">
         <v>21</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G44" s="6">
+      <c r="C45" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="14">
         <v>44378</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
-      <c r="G45" s="5"/>
-    </row>
     <row r="46" spans="1:8">
-      <c r="A46" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="5">
-        <v>15.1</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46" s="6">
-        <v>44203</v>
-      </c>
+      <c r="G46" s="14"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B47" s="5">
-        <v>15.2</v>
+        <v>15.1</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D47" s="5"/>
       <c r="E47" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G47" s="6"/>
-    </row>
-    <row r="48" spans="1:8" ht="30">
+      <c r="G47" s="14">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B48" s="5">
-        <v>15.3</v>
+        <v>15.2</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="5"/>
       <c r="E48" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G48" s="6">
+      <c r="G48" s="14"/>
+    </row>
+    <row r="49" spans="1:8" ht="30">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="5">
+        <v>15.3</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="14">
         <v>44316</v>
       </c>
-      <c r="H48" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
+      <c r="H49" s="13" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G50" s="6">
-        <v>44392</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>93</v>
-      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="14"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>38</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>52</v>
+        <v>11</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" s="6">
-        <v>44187</v>
+        <v>98</v>
+      </c>
+      <c r="G51" s="14">
+        <v>44392</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>38</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>51</v>
+        <v>36</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G52" s="6">
-        <v>44393</v>
-      </c>
-      <c r="H52" s="9"/>
+        <v>98</v>
+      </c>
+      <c r="G52" s="14">
+        <v>44187</v>
+      </c>
+      <c r="H52" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="8">
-        <v>21.04</v>
+        <v>36</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" s="6">
-        <v>44203</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="G53" s="14">
+        <v>44393</v>
+      </c>
+      <c r="H53" s="9"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="8">
+        <v>21.04</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D54" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G54" s="6">
+        <v>98</v>
+      </c>
+      <c r="G54" s="14">
         <v>44203</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" s="5">
+        <v>13</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G55" s="14">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="5">
         <v>20.12</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G55" s="6">
+      <c r="C56" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G56" s="14">
         <v>44215</v>
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" t="s">
-        <v>69</v>
-      </c>
-      <c r="B57" s="8">
-        <v>12.2</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G57" s="6">
-        <v>44294</v>
-      </c>
-      <c r="H57" s="12" t="s">
-        <v>73</v>
-      </c>
+      <c r="G57" s="14"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B58" s="8">
         <v>12.2</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G58" s="6">
+        <v>101</v>
+      </c>
+      <c r="G58" s="14">
         <v>44294</v>
       </c>
-      <c r="H58" s="12"/>
+      <c r="H58" s="12" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>69</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
+      </c>
+      <c r="B59" s="8">
+        <v>12.2</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G59" s="6">
-        <v>44298</v>
+        <v>65</v>
+      </c>
+      <c r="G59" s="14">
+        <v>44480</v>
       </c>
       <c r="H59" s="12"/>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G60" s="14">
+        <v>44298</v>
+      </c>
+      <c r="H60" s="12"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B60" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C60" s="5" t="s">
+      <c r="C61" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G61" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" t="s">
-        <v>78</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G62" s="6">
-        <v>44383</v>
-      </c>
-      <c r="H62" t="s">
-        <v>81</v>
-      </c>
+      <c r="G62" s="14"/>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>78</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G63" s="6">
-        <v>44318</v>
+      <c r="G63" s="14">
+        <v>44383</v>
       </c>
       <c r="H63" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64" s="14">
+        <v>44318</v>
+      </c>
+      <c r="H64" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65" s="8">
+        <v>10.15</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" s="14"/>
+      <c r="H65" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="8">
-        <v>10.15</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G64" s="6"/>
-      <c r="H64" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" t="s">
-        <v>78</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G65" s="6">
-        <v>44409</v>
-      </c>
-      <c r="H65" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>78</v>
-      </c>
-      <c r="B66" s="5">
+        <v>73</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G66" s="14">
+        <v>44436</v>
+      </c>
+      <c r="H66" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" s="14">
+        <v>44436</v>
+      </c>
+      <c r="H67" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68" s="5">
+        <v>12</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G68" s="14">
+        <v>44470</v>
+      </c>
+      <c r="H68" t="s">
+        <v>104</v>
+      </c>
+      <c r="I68" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69" s="5">
         <v>11.4</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G66" s="6">
+      <c r="C69" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G69" s="14">
         <v>44383</v>
       </c>
-      <c r="H66" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="B67" s="5"/>
+      <c r="H69" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="B70" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Update test matrix to show Manjaro
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="test-matrix" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="110">
   <si>
     <t>CentOS</t>
   </si>
@@ -132,9 +132,6 @@
     <t>armv7l</t>
   </si>
   <si>
-    <t>VMware indicates VMware 15.5 running on Windows 10 running on Intel i7 CPU</t>
-  </si>
-  <si>
     <t>Target OS</t>
   </si>
   <si>
@@ -144,18 +141,12 @@
     <t>OS Version</t>
   </si>
   <si>
-    <t>Target CPU Architecture</t>
-  </si>
-  <si>
     <t>All builds are compiled natively on the target OS (not cross compiled)</t>
   </si>
   <si>
     <t>All builds match the bitness of the installed OS</t>
   </si>
   <si>
-    <t>System Hardware</t>
-  </si>
-  <si>
     <t>gcc 5.4.0</t>
   </si>
   <si>
@@ -174,9 +165,6 @@
     <t>openSUSE</t>
   </si>
   <si>
-    <t>RAM Size</t>
-  </si>
-  <si>
     <t>2 GB</t>
   </si>
   <si>
@@ -300,9 +288,6 @@
     <t>Zorin</t>
   </si>
   <si>
-    <t>11.15.1</t>
-  </si>
-  <si>
     <t>seems to be based on Ubuntu 18.04</t>
   </si>
   <si>
@@ -333,9 +318,6 @@
     <t>Monterey (Beta)</t>
   </si>
   <si>
-    <t>under construction</t>
-  </si>
-  <si>
     <t>Arch</t>
   </si>
   <si>
@@ -343,6 +325,27 @@
   </si>
   <si>
     <t>gcc 11.1.0</t>
+  </si>
+  <si>
+    <t>11.5.1</t>
+  </si>
+  <si>
+    <t>21 5.10.136</t>
+  </si>
+  <si>
+    <t>gcc 12.1.1</t>
+  </si>
+  <si>
+    <t>VMware indicates VMware 16.2.3 running on Windows 10 running on Intel i7 CPU</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>System</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -432,9 +435,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -734,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I70"/>
+  <dimension ref="A2:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -763,7 +763,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44483</v>
+        <v>44816</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -776,47 +776,47 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="B10" s="2"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="30.75" customHeight="1">
+    <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>28</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>3</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -828,24 +828,24 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G13" s="14">
+      <c r="G13" s="13">
         <v>44252</v>
       </c>
     </row>
@@ -855,11 +855,11 @@
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="14"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B15" s="5">
         <v>8.4</v>
@@ -868,15 +868,15 @@
         <v>5</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="13">
         <v>44393</v>
       </c>
     </row>
@@ -885,19 +885,19 @@
         <v>0</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="13">
         <v>44210</v>
       </c>
     </row>
@@ -918,7 +918,7 @@
       <c r="F17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="13">
         <v>44210</v>
       </c>
     </row>
@@ -939,13 +939,13 @@
       <c r="F18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <v>44210</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B19" s="5">
         <v>34</v>
@@ -954,15 +954,15 @@
         <v>5</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="13">
         <v>44378</v>
       </c>
     </row>
@@ -971,20 +971,20 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="14"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>21</v>
@@ -992,7 +992,7 @@
       <c r="F21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="13">
         <v>44377</v>
       </c>
     </row>
@@ -1004,7 +1004,7 @@
         <v>10.6</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
@@ -1013,7 +1013,7 @@
       <c r="F22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="13">
         <v>44187</v>
       </c>
     </row>
@@ -1025,7 +1025,7 @@
         <v>9.9</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
@@ -1034,7 +1034,7 @@
       <c r="F23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="13">
         <v>44177</v>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
         <v>8.6</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
@@ -1055,7 +1055,7 @@
       <c r="F24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="13">
         <v>44183</v>
       </c>
       <c r="H24" s="9"/>
@@ -1068,7 +1068,7 @@
         <v>8.6</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
@@ -1077,7 +1077,7 @@
       <c r="F25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="13">
         <v>44182</v>
       </c>
       <c r="H25" s="9"/>
@@ -1090,16 +1090,16 @@
         <v>8.6</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="13">
         <v>44185</v>
       </c>
       <c r="H26" s="9" t="s">
@@ -1114,7 +1114,7 @@
         <v>8.6</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="s">
@@ -1123,7 +1123,7 @@
       <c r="F27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="13">
         <v>44177</v>
       </c>
       <c r="H27" s="9" t="s">
@@ -1138,7 +1138,7 @@
         <v>8.6</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
@@ -1147,7 +1147,7 @@
       <c r="F28" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="13">
         <v>44177</v>
       </c>
       <c r="H28" s="9" t="s">
@@ -1160,12 +1160,12 @@
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="14"/>
+      <c r="G29" s="13"/>
       <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B30" s="5">
         <v>15.3</v>
@@ -1174,7 +1174,7 @@
         <v>5</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>24</v>
@@ -1182,16 +1182,16 @@
       <c r="F30" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="13">
         <v>44378</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B31" s="5">
         <v>20.04</v>
@@ -1206,7 +1206,7 @@
       <c r="F31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="13">
         <v>44411</v>
       </c>
       <c r="H31" s="9"/>
@@ -1228,7 +1228,7 @@
       <c r="F32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="13">
         <v>44178</v>
       </c>
     </row>
@@ -1249,7 +1249,7 @@
       <c r="F33" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="13">
         <v>44177</v>
       </c>
     </row>
@@ -1265,16 +1265,16 @@
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G34" s="14">
+        <v>55</v>
+      </c>
+      <c r="G34" s="13">
         <v>44245</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1285,7 +1285,7 @@
         <v>12.04</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
@@ -1294,7 +1294,7 @@
       <c r="F35" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="13">
         <v>44183</v>
       </c>
       <c r="H35" s="9"/>
@@ -1307,7 +1307,7 @@
         <v>12.04</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
@@ -1316,7 +1316,7 @@
       <c r="F36" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="13">
         <v>44182</v>
       </c>
       <c r="H36" s="9"/>
@@ -1329,7 +1329,7 @@
         <v>12.04</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="s">
@@ -1338,7 +1338,7 @@
       <c r="F37" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="13">
         <v>44177</v>
       </c>
       <c r="H37" s="9" t="s">
@@ -1353,7 +1353,7 @@
         <v>12.04</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
@@ -1362,7 +1362,7 @@
       <c r="F38" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G38" s="13">
         <v>44177</v>
       </c>
       <c r="H38" s="9" t="s">
@@ -1374,7 +1374,7 @@
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="14"/>
+      <c r="G39" s="13"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
@@ -1387,7 +1387,7 @@
         <v>5</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>26</v>
@@ -1395,7 +1395,7 @@
       <c r="F40" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="13">
         <v>44383</v>
       </c>
     </row>
@@ -1410,7 +1410,7 @@
         <v>5</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>26</v>
@@ -1418,7 +1418,7 @@
       <c r="F41" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="13">
         <v>44205</v>
       </c>
     </row>
@@ -1439,7 +1439,7 @@
       <c r="F42" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="14">
+      <c r="G42" s="13">
         <v>44177</v>
       </c>
     </row>
@@ -1460,60 +1460,62 @@
       <c r="F43" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G43" s="14">
+      <c r="G43" s="13">
         <v>44178</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G44" s="14">
+      <c r="G44" s="13">
         <v>44483</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>92</v>
-      </c>
-      <c r="B45" s="5">
-        <v>21</v>
+        <v>88</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E45" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>105</v>
+      </c>
       <c r="F45" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G45" s="14">
-        <v>44378</v>
+      <c r="G45" s="13">
+        <v>44816</v>
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="G46" s="14"/>
+      <c r="G46" s="13"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B47" s="5">
         <v>15.1</v>
@@ -1528,13 +1530,13 @@
       <c r="F47" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G47" s="14">
+      <c r="G47" s="13">
         <v>44203</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B48" s="5">
         <v>15.2</v>
@@ -1549,11 +1551,11 @@
       <c r="F48" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G48" s="14"/>
-    </row>
-    <row r="49" spans="1:8" ht="30">
+      <c r="G48" s="13"/>
+    </row>
+    <row r="49" spans="1:8" ht="15" customHeight="1">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B49" s="5">
         <v>15.3</v>
@@ -1568,11 +1570,11 @@
       <c r="F49" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G49" s="14">
+      <c r="G49" s="13">
         <v>44316</v>
       </c>
-      <c r="H49" s="13" t="s">
-        <v>87</v>
+      <c r="H49" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1581,7 +1583,7 @@
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
-      <c r="G50" s="14"/>
+      <c r="G50" s="13"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
@@ -1594,19 +1596,19 @@
         <v>14</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G51" s="14">
+        <v>93</v>
+      </c>
+      <c r="G51" s="13">
         <v>44392</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1614,21 +1616,21 @@
         <v>36</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G52" s="14">
+        <v>93</v>
+      </c>
+      <c r="G52" s="13">
         <v>44187</v>
       </c>
       <c r="H52" s="9" t="s">
@@ -1640,21 +1642,21 @@
         <v>36</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G53" s="14">
+        <v>94</v>
+      </c>
+      <c r="G53" s="13">
         <v>44393</v>
       </c>
       <c r="H53" s="9"/>
@@ -1670,15 +1672,15 @@
         <v>14</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G54" s="14">
+        <v>93</v>
+      </c>
+      <c r="G54" s="13">
         <v>44203</v>
       </c>
     </row>
@@ -1693,21 +1695,21 @@
         <v>14</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G55" s="14">
+        <v>95</v>
+      </c>
+      <c r="G55" s="13">
         <v>44203</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B56" s="5">
         <v>20.12</v>
@@ -1716,47 +1718,47 @@
         <v>14</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G56" s="14">
+        <v>95</v>
+      </c>
+      <c r="G56" s="13">
         <v>44215</v>
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="G57" s="14"/>
+      <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B58" s="8">
         <v>12.2</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G58" s="14">
+        <v>96</v>
+      </c>
+      <c r="G58" s="13">
         <v>44294</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B59" s="8">
         <v>12.2</v>
@@ -1765,33 +1767,33 @@
         <v>5</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G59" s="14">
+        <v>61</v>
+      </c>
+      <c r="G59" s="13">
         <v>44480</v>
       </c>
       <c r="H59" s="12"/>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="C60" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E60" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="F60" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G60" s="14">
+        <v>97</v>
+      </c>
+      <c r="G60" s="13">
         <v>44298</v>
       </c>
       <c r="H60" s="12"/>
@@ -1809,64 +1811,64 @@
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G61" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G61" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="G62" s="14"/>
+      <c r="G62" s="13"/>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G63" s="14">
+      <c r="G63" s="13">
         <v>44383</v>
       </c>
       <c r="H63" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G64" s="14">
+      <c r="G64" s="13">
         <v>44318</v>
       </c>
       <c r="H64" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B65" s="8">
         <v>10.15</v>
@@ -1878,60 +1880,60 @@
       <c r="F65" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G65" s="14"/>
+      <c r="G65" s="13"/>
       <c r="H65" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G66" s="14">
+      <c r="G66" s="13">
         <v>44436</v>
       </c>
       <c r="H66" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G67" s="14">
+      <c r="G67" s="13">
         <v>44436</v>
       </c>
       <c r="H67" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B68" s="5">
         <v>12</v>
@@ -1940,45 +1942,42 @@
         <v>33</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G68" s="14">
+      <c r="G68" s="13">
         <v>44470</v>
       </c>
       <c r="H68" t="s">
-        <v>104</v>
-      </c>
-      <c r="I68" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B69" s="5">
         <v>11.4</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G69" s="14">
+        <v>77</v>
+      </c>
+      <c r="G69" s="13">
         <v>44383</v>
       </c>
       <c r="H69" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
       <c r="B70" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test matrix to show Fedora 36
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -261,9 +261,6 @@
     <t>Fedora</t>
   </si>
   <si>
-    <t>gcc 11.1.1</t>
-  </si>
-  <si>
     <t>AlmaLinux</t>
   </si>
   <si>
@@ -346,6 +343,9 @@
   </si>
   <si>
     <t>System</t>
+  </si>
+  <si>
+    <t>gcc 12.2.1</t>
   </si>
 </sst>
 </file>
@@ -737,7 +737,7 @@
   <dimension ref="A2:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -776,7 +776,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -801,16 +801,16 @@
         <v>40</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>107</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>108</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>28</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>3</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" s="5">
         <v>8.4</v>
@@ -948,7 +948,7 @@
         <v>80</v>
       </c>
       <c r="B19" s="5">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>5</v>
@@ -957,13 +957,13 @@
         <v>50</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="13">
-        <v>44378</v>
+        <v>37480</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1004,7 +1004,7 @@
         <v>10.6</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
@@ -1025,7 +1025,7 @@
         <v>9.9</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
@@ -1046,7 +1046,7 @@
         <v>8.6</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
@@ -1068,7 +1068,7 @@
         <v>8.6</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
@@ -1090,7 +1090,7 @@
         <v>8.6</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
@@ -1114,7 +1114,7 @@
         <v>8.6</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="s">
@@ -1138,7 +1138,7 @@
         <v>8.6</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
@@ -1165,7 +1165,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="5">
         <v>15.3</v>
@@ -1186,7 +1186,7 @@
         <v>44378</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1285,7 +1285,7 @@
         <v>12.04</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
@@ -1307,7 +1307,7 @@
         <v>12.04</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
@@ -1329,7 +1329,7 @@
         <v>12.04</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="s">
@@ -1353,7 +1353,7 @@
         <v>12.04</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
@@ -1466,10 +1466,10 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>5</v>
@@ -1478,7 +1478,7 @@
         <v>50</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>9</v>
@@ -1489,10 +1489,10 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>5</v>
@@ -1501,7 +1501,7 @@
         <v>50</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>9</v>
@@ -1574,7 +1574,7 @@
         <v>44316</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1596,19 +1596,19 @@
         <v>14</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G51" s="13">
         <v>44392</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1622,13 +1622,13 @@
         <v>37</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G52" s="13">
         <v>44187</v>
@@ -1648,13 +1648,13 @@
         <v>44</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G53" s="13">
         <v>44393</v>
@@ -1672,13 +1672,13 @@
         <v>14</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G54" s="13">
         <v>44203</v>
@@ -1695,13 +1695,13 @@
         <v>14</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G55" s="13">
         <v>44203</v>
@@ -1718,13 +1718,13 @@
         <v>14</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G56" s="13">
         <v>44215</v>
@@ -1747,7 +1747,7 @@
         <v>64</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G58" s="13">
         <v>44294</v>
@@ -1791,7 +1791,7 @@
         <v>67</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G60" s="13">
         <v>44298</v>
@@ -1890,7 +1890,7 @@
         <v>69</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>33</v>
@@ -1905,7 +1905,7 @@
         <v>44436</v>
       </c>
       <c r="H66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -1913,7 +1913,7 @@
         <v>69</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>33</v>
@@ -1928,7 +1928,7 @@
         <v>44436</v>
       </c>
       <c r="H67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -1942,7 +1942,7 @@
         <v>33</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>9</v>
@@ -1951,7 +1951,7 @@
         <v>44470</v>
       </c>
       <c r="H68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:8">

</xml_diff>

<commit_message>
Update test matrix for Debian 32-bit and RPIOS 32-bit
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="112">
   <si>
     <t>CentOS</t>
   </si>
@@ -346,6 +346,12 @@
   </si>
   <si>
     <t>gcc 12.2.1</t>
+  </si>
+  <si>
+    <t>clang 7.0.1</t>
+  </si>
+  <si>
+    <t>Build fails: missing __atomic_compare_exchange_8</t>
   </si>
 </sst>
 </file>
@@ -734,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H70"/>
+  <dimension ref="A2:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -748,7 +754,7 @@
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
     <col min="5" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="8" max="8" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8">
@@ -763,7 +769,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44816</v>
+        <v>44817</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -963,7 +969,7 @@
         <v>9</v>
       </c>
       <c r="G19" s="13">
-        <v>37480</v>
+        <v>44817</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1006,7 +1012,9 @@
       <c r="C22" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E22" s="5" t="s">
         <v>21</v>
       </c>
@@ -1014,7 +1022,7 @@
         <v>9</v>
       </c>
       <c r="G22" s="13">
-        <v>44187</v>
+        <v>44817</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1022,20 +1030,25 @@
         <v>1</v>
       </c>
       <c r="B23" s="5">
-        <v>9.9</v>
+        <v>10.6</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E23" s="5" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="13">
-        <v>44177</v>
+        <v>44817</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1043,22 +1056,21 @@
         <v>1</v>
       </c>
       <c r="B24" s="5">
-        <v>8.6</v>
+        <v>9.9</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>86</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G24" s="13">
-        <v>44183</v>
-      </c>
-      <c r="H24" s="9"/>
+        <v>44177</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
@@ -1072,13 +1084,13 @@
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="13">
-        <v>44182</v>
+        <v>44183</v>
       </c>
       <c r="H25" s="9"/>
     </row>
@@ -1094,17 +1106,15 @@
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G26" s="13">
-        <v>44185</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>44182</v>
+      </c>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
@@ -1118,13 +1128,13 @@
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G27" s="13">
-        <v>44177</v>
+        <v>44185</v>
       </c>
       <c r="H27" s="9" t="s">
         <v>30</v>
@@ -1142,7 +1152,7 @@
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>9</v>
@@ -1151,69 +1161,71 @@
         <v>44177</v>
       </c>
       <c r="H28" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="5">
+        <v>8.6</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="13">
+        <v>44177</v>
+      </c>
+      <c r="H29" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="9"/>
-    </row>
     <row r="30" spans="1:8">
-      <c r="A30" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" s="5">
-        <v>15.3</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="13">
-        <v>44378</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>89</v>
-      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="B31" s="5">
-        <v>20.04</v>
+        <v>15.3</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="E31" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G31" s="13">
-        <v>44411</v>
-      </c>
-      <c r="H31" s="9"/>
+        <v>44378</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B32" s="5">
         <v>20.04</v>
@@ -1226,31 +1238,32 @@
         <v>26</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G32" s="13">
-        <v>44178</v>
-      </c>
+        <v>44411</v>
+      </c>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>6</v>
       </c>
       <c r="B33" s="5">
-        <v>18.04</v>
+        <v>20.04</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G33" s="13">
-        <v>44177</v>
+        <v>44178</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1258,23 +1271,20 @@
         <v>6</v>
       </c>
       <c r="B34" s="5">
-        <v>16.04</v>
+        <v>18.04</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="G34" s="13">
-        <v>44245</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>54</v>
+        <v>44177</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1282,22 +1292,24 @@
         <v>6</v>
       </c>
       <c r="B35" s="5">
-        <v>12.04</v>
+        <v>16.04</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="G35" s="13">
-        <v>44183</v>
-      </c>
-      <c r="H35" s="9"/>
+        <v>44245</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
@@ -1311,13 +1323,13 @@
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G36" s="13">
-        <v>44182</v>
+        <v>44183</v>
       </c>
       <c r="H36" s="9"/>
     </row>
@@ -1333,17 +1345,15 @@
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G37" s="13">
-        <v>44177</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>44182</v>
+      </c>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
@@ -1357,7 +1367,7 @@
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>9</v>
@@ -1370,47 +1380,48 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="13"/>
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="5">
+        <v>12.04</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="13">
+        <v>44177</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="5">
-        <v>5.21</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G40" s="13">
-        <v>44383</v>
-      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="13"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>10</v>
       </c>
       <c r="B41" s="5">
-        <v>20.04</v>
+        <v>5.21</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>26</v>
@@ -1419,7 +1430,7 @@
         <v>9</v>
       </c>
       <c r="G41" s="13">
-        <v>44205</v>
+        <v>44383</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1427,72 +1438,72 @@
         <v>10</v>
       </c>
       <c r="B42" s="5">
-        <v>11.19</v>
+        <v>20.04</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="5"/>
+      <c r="D42" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="E42" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G42" s="13">
-        <v>44177</v>
+        <v>44205</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B43" s="5">
-        <v>20</v>
+        <v>11.19</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G43" s="13">
-        <v>44178</v>
+        <v>44177</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>99</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>100</v>
+        <v>8</v>
+      </c>
+      <c r="B44" s="5">
+        <v>20</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="D44" s="5"/>
       <c r="E44" s="5" t="s">
-        <v>101</v>
+        <v>26</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G44" s="13">
-        <v>44483</v>
+        <v>44178</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>5</v>
@@ -1501,45 +1512,47 @@
         <v>50</v>
       </c>
       <c r="E45" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="13">
+        <v>44483</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>87</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F45" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G45" s="13">
+      <c r="F46" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="13">
         <v>44816</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
-      <c r="G46" s="13"/>
-    </row>
     <row r="47" spans="1:8">
-      <c r="A47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="5">
-        <v>15.1</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G47" s="13">
-        <v>44203</v>
-      </c>
+      <c r="G47" s="13"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48" s="5">
-        <v>15.2</v>
+        <v>15.1</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>5</v>
@@ -1551,14 +1564,16 @@
       <c r="F48" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G48" s="13"/>
-    </row>
-    <row r="49" spans="1:8" ht="15" customHeight="1">
+      <c r="G48" s="13">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="5">
-        <v>15.3</v>
+        <v>15.2</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>5</v>
@@ -1570,56 +1585,49 @@
       <c r="F49" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G49" s="13">
+      <c r="G49" s="13"/>
+    </row>
+    <row r="50" spans="1:8" ht="15" customHeight="1">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="5">
+        <v>15.3</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="13">
         <v>44316</v>
       </c>
-      <c r="H49" s="9" t="s">
+      <c r="H50" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="13"/>
-    </row>
     <row r="51" spans="1:8">
-      <c r="A51" t="s">
-        <v>11</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G51" s="13">
-        <v>44392</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>83</v>
-      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="13"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>36</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>46</v>
+        <v>11</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>84</v>
@@ -1631,65 +1639,68 @@
         <v>92</v>
       </c>
       <c r="G52" s="13">
-        <v>44187</v>
+        <v>44392</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>36</v>
       </c>
-      <c r="B53" s="6" t="s">
-        <v>45</v>
+      <c r="B53" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G53" s="13">
-        <v>44393</v>
-      </c>
-      <c r="H53" s="9"/>
+        <v>44817</v>
+      </c>
+      <c r="H53" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" s="8">
-        <v>21.04</v>
+        <v>36</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G54" s="13">
-        <v>44203</v>
-      </c>
+        <v>44393</v>
+      </c>
+      <c r="H54" s="9"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="B55" s="8">
+        <v>21.04</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>14</v>
@@ -1698,10 +1709,10 @@
         <v>84</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G55" s="13">
         <v>44203</v>
@@ -1709,10 +1720,10 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>53</v>
-      </c>
-      <c r="B56" s="5">
-        <v>20.12</v>
+        <v>13</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>14</v>
@@ -1727,34 +1738,34 @@
         <v>94</v>
       </c>
       <c r="G56" s="13">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" s="5">
+        <v>20.12</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G57" s="13">
         <v>44215</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
-      <c r="G57" s="13"/>
-    </row>
     <row r="58" spans="1:8">
-      <c r="A58" t="s">
-        <v>62</v>
-      </c>
-      <c r="B58" s="8">
-        <v>12.2</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G58" s="13">
-        <v>44294</v>
-      </c>
-      <c r="H58" s="12" t="s">
-        <v>65</v>
-      </c>
+      <c r="G58" s="13"/>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
@@ -1764,148 +1775,148 @@
         <v>12.2</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>64</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="G59" s="13">
-        <v>44480</v>
-      </c>
-      <c r="H59" s="12"/>
+        <v>44294</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>62</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>66</v>
+      <c r="B60" s="8">
+        <v>12.2</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="G60" s="13">
-        <v>44298</v>
+        <v>44480</v>
       </c>
       <c r="H60" s="12"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G61" s="13">
+        <v>44298</v>
+      </c>
+      <c r="H61" s="12"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B62" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C62" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5" t="s">
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G61" s="13" t="s">
+      <c r="G62" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
-      <c r="G62" s="13"/>
-    </row>
     <row r="63" spans="1:8">
-      <c r="A63" t="s">
-        <v>69</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G63" s="13">
-        <v>44383</v>
-      </c>
-      <c r="H63" t="s">
-        <v>72</v>
-      </c>
+      <c r="G63" s="13"/>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>69</v>
       </c>
-      <c r="B64" s="8" t="s">
-        <v>70</v>
+      <c r="B64" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G64" s="13">
-        <v>44318</v>
+        <v>44383</v>
       </c>
       <c r="H64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>69</v>
       </c>
-      <c r="B65" s="8">
-        <v>10.15</v>
+      <c r="B65" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E65" s="5"/>
+      <c r="E65" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="F65" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G65" s="13"/>
+      <c r="G65" s="13">
+        <v>44318</v>
+      </c>
       <c r="H65" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>69</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>102</v>
+      <c r="B66" s="8">
+        <v>10.15</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E66" s="5" t="s">
-        <v>78</v>
-      </c>
+      <c r="E66" s="5"/>
       <c r="F66" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G66" s="13">
-        <v>44436</v>
-      </c>
+      <c r="G66" s="13"/>
       <c r="H66" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -1928,30 +1939,30 @@
         <v>44436</v>
       </c>
       <c r="H67" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="5">
-        <v>12</v>
+      <c r="B68" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G68" s="13">
-        <v>44470</v>
+        <v>44436</v>
       </c>
       <c r="H68" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -1959,26 +1970,49 @@
         <v>69</v>
       </c>
       <c r="B69" s="5">
+        <v>12</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G69" s="13">
+        <v>44470</v>
+      </c>
+      <c r="H69" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="5">
         <v>11.4</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C70" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="E70" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="F70" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G69" s="13">
+      <c r="G70" s="13">
         <v>44383</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H70" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
-      <c r="B70" s="5"/>
+    <row r="71" spans="1:8">
+      <c r="B71" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Update test matrix for Ubuntu 22.10 with gcc 12.2.0
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="116">
   <si>
     <t>CentOS</t>
   </si>
@@ -333,9 +333,6 @@
     <t>gcc 12.1.1</t>
   </si>
   <si>
-    <t>VMware indicates VMware 16.2.3 running on Windows 10 running on Intel i7 CPU</t>
-  </si>
-  <si>
     <t>CPU</t>
   </si>
   <si>
@@ -352,6 +349,21 @@
   </si>
   <si>
     <t>Build fails: missing __atomic_compare_exchange_8</t>
+  </si>
+  <si>
+    <t>gcc 10.2.1</t>
+  </si>
+  <si>
+    <t>OpenBSD</t>
+  </si>
+  <si>
+    <t>trouble with dlopen()</t>
+  </si>
+  <si>
+    <t>VMware indicates VMware 16 running on Windows 10 running on Intel i7 CPU</t>
+  </si>
+  <si>
+    <t>gcc 12.2.0</t>
   </si>
 </sst>
 </file>
@@ -410,7 +422,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -443,6 +455,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -740,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H71"/>
+  <dimension ref="A2:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -769,7 +784,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44817</v>
+        <v>44855</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -782,7 +797,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -807,16 +822,16 @@
         <v>40</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>107</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>28</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>3</v>
@@ -963,7 +978,7 @@
         <v>50</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>9</v>
@@ -983,34 +998,34 @@
       <c r="A21" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>68</v>
+      <c r="B21" s="8">
+        <v>11</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G21" s="13">
-        <v>44377</v>
+        <v>44817</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="5">
-        <v>10.6</v>
+      <c r="B22" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>59</v>
@@ -1039,16 +1054,13 @@
         <v>59</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="13">
         <v>44817</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1056,20 +1068,25 @@
         <v>1</v>
       </c>
       <c r="B24" s="5">
-        <v>9.9</v>
+        <v>10.6</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E24" s="5" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G24" s="13">
-        <v>44177</v>
+        <v>44817</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1077,22 +1094,21 @@
         <v>1</v>
       </c>
       <c r="B25" s="5">
-        <v>8.6</v>
+        <v>9.9</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>86</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="13">
-        <v>44183</v>
-      </c>
-      <c r="H25" s="9"/>
+        <v>44177</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
@@ -1106,13 +1122,13 @@
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G26" s="13">
-        <v>44182</v>
+        <v>44183</v>
       </c>
       <c r="H26" s="9"/>
     </row>
@@ -1128,17 +1144,15 @@
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G27" s="13">
-        <v>44185</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>44182</v>
+      </c>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
@@ -1152,13 +1166,13 @@
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G28" s="13">
-        <v>44177</v>
+        <v>44185</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>30</v>
@@ -1176,7 +1190,7 @@
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>9</v>
@@ -1185,69 +1199,71 @@
         <v>44177</v>
       </c>
       <c r="H29" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="5">
+        <v>8.6</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="13">
+        <v>44177</v>
+      </c>
+      <c r="H30" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="9"/>
-    </row>
     <row r="31" spans="1:8">
-      <c r="A31" t="s">
-        <v>88</v>
-      </c>
-      <c r="B31" s="5">
-        <v>15.3</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="13">
-        <v>44378</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>89</v>
-      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="B32" s="5">
-        <v>20.04</v>
+        <v>15.3</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="E32" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G32" s="13">
-        <v>44411</v>
-      </c>
-      <c r="H32" s="9"/>
+        <v>44378</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B33" s="5">
         <v>20.04</v>
@@ -1260,31 +1276,34 @@
         <v>26</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G33" s="13">
-        <v>44178</v>
-      </c>
+        <v>44411</v>
+      </c>
+      <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="5">
-        <v>18.04</v>
+      <c r="B34" s="14">
+        <v>22.1</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="5"/>
+      <c r="D34" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E34" s="5" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G34" s="13">
-        <v>44177</v>
+        <v>44855</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1292,23 +1311,20 @@
         <v>6</v>
       </c>
       <c r="B35" s="5">
-        <v>16.04</v>
+        <v>20.04</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="G35" s="13">
-        <v>44245</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>54</v>
+        <v>44178</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1316,44 +1332,45 @@
         <v>6</v>
       </c>
       <c r="B36" s="5">
-        <v>12.04</v>
+        <v>18.04</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G36" s="13">
-        <v>44183</v>
-      </c>
-      <c r="H36" s="9"/>
+        <v>44177</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>6</v>
       </c>
       <c r="B37" s="5">
-        <v>12.04</v>
+        <v>16.04</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="G37" s="13">
-        <v>44182</v>
-      </c>
-      <c r="H37" s="9"/>
+        <v>44245</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
@@ -1367,17 +1384,15 @@
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G38" s="13">
-        <v>44177</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>44183</v>
+      </c>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
@@ -1391,103 +1406,107 @@
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G39" s="13">
+        <v>44182</v>
+      </c>
+      <c r="H39" s="9"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="5">
+        <v>12.04</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="13">
         <v>44177</v>
       </c>
-      <c r="H39" s="9" t="s">
+      <c r="H40" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="13"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B41" s="5">
-        <v>5.21</v>
+        <v>12.04</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G41" s="13">
-        <v>44383</v>
+        <v>44177</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="5">
-        <v>20.04</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G42" s="13">
-        <v>44205</v>
-      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="13"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>10</v>
       </c>
       <c r="B43" s="5">
-        <v>11.19</v>
+        <v>5.21</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="5"/>
+      <c r="D43" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E43" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G43" s="13">
-        <v>44177</v>
+        <v>44383</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B44" s="5">
-        <v>20</v>
+        <v>20.04</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="5"/>
+      <c r="D44" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="E44" s="5" t="s">
         <v>26</v>
       </c>
@@ -1495,104 +1514,106 @@
         <v>9</v>
       </c>
       <c r="G44" s="13">
-        <v>44178</v>
+        <v>44205</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>100</v>
+        <v>10</v>
+      </c>
+      <c r="B45" s="5">
+        <v>11.19</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
-        <v>101</v>
+        <v>24</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G45" s="13">
-        <v>44483</v>
+        <v>44177</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>103</v>
+        <v>8</v>
+      </c>
+      <c r="B46" s="5">
+        <v>20</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="5"/>
+      <c r="E46" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="13">
+        <v>44178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46" s="13">
-        <v>44816</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="G47" s="13"/>
+      <c r="E47" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="13">
+        <v>44483</v>
+      </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" s="5">
-        <v>15.1</v>
+        <v>87</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="5"/>
+      <c r="D48" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="E48" s="5" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G48" s="13">
-        <v>44203</v>
+        <v>44816</v>
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" s="5">
-        <v>15.2</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="G49" s="13"/>
     </row>
-    <row r="50" spans="1:8" ht="15" customHeight="1">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>48</v>
       </c>
       <c r="B50" s="5">
-        <v>15.3</v>
+        <v>15.1</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>5</v>
@@ -1605,148 +1626,142 @@
         <v>9</v>
       </c>
       <c r="G50" s="13">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="5">
+        <v>15.2</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" s="13"/>
+    </row>
+    <row r="52" spans="1:8" ht="15" customHeight="1">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="5">
+        <v>15.3</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" s="13">
         <v>44316</v>
       </c>
-      <c r="H50" s="9" t="s">
+      <c r="H52" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="13"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" t="s">
-        <v>11</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G52" s="13">
-        <v>44392</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
     <row r="53" spans="1:8">
-      <c r="A53" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G53" s="13">
-        <v>44817</v>
-      </c>
-      <c r="H53" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="13"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>45</v>
+        <v>11</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G54" s="13">
-        <v>44393</v>
-      </c>
-      <c r="H54" s="9"/>
+        <v>44392</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55" s="8">
-        <v>21.04</v>
+        <v>36</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>84</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>92</v>
       </c>
       <c r="G55" s="13">
-        <v>44203</v>
+        <v>44817</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>13</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G56" s="13">
-        <v>44203</v>
-      </c>
+        <v>44393</v>
+      </c>
+      <c r="H56" s="9"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>53</v>
-      </c>
-      <c r="B57" s="5">
-        <v>20.12</v>
+        <v>6</v>
+      </c>
+      <c r="B57" s="8">
+        <v>21.04</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>14</v>
@@ -1755,264 +1770,336 @@
         <v>84</v>
       </c>
       <c r="E57" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G57" s="13">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="F58" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G57" s="13">
-        <v>44215</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="G58" s="13"/>
+      <c r="G58" s="13">
+        <v>44203</v>
+      </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>62</v>
-      </c>
-      <c r="B59" s="8">
-        <v>12.2</v>
+        <v>53</v>
+      </c>
+      <c r="B59" s="5">
+        <v>20.12</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>63</v>
+        <v>14</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G59" s="13">
-        <v>44294</v>
-      </c>
-      <c r="H59" s="12" t="s">
-        <v>65</v>
+        <v>44215</v>
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" t="s">
-        <v>62</v>
-      </c>
-      <c r="B60" s="8">
-        <v>12.2</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G60" s="13">
-        <v>44480</v>
-      </c>
-      <c r="H60" s="12"/>
+      <c r="G60" s="13"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>62</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>66</v>
+      <c r="B61" s="8">
+        <v>12.2</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>63</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G61" s="13">
-        <v>44298</v>
-      </c>
-      <c r="H61" s="12"/>
+        <v>44294</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>32</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>34</v>
+        <v>62</v>
+      </c>
+      <c r="B62" s="8">
+        <v>12.2</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="F62" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G62" s="13" t="s">
-        <v>35</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="G62" s="13">
+        <v>44480</v>
+      </c>
+      <c r="H62" s="12"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="G63" s="13"/>
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G63" s="13">
+        <v>44298</v>
+      </c>
+      <c r="H63" s="12"/>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>69</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>71</v>
+        <v>32</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E64" s="5" t="s">
-        <v>79</v>
-      </c>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
       <c r="F64" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G64" s="13">
-        <v>44383</v>
-      </c>
-      <c r="H64" t="s">
-        <v>72</v>
+        <v>39</v>
+      </c>
+      <c r="G64" s="13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>70</v>
+        <v>112</v>
+      </c>
+      <c r="B65" s="8">
+        <v>7.1</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="D65" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E65" s="5" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G65" s="13">
-        <v>44318</v>
-      </c>
-      <c r="H65" t="s">
-        <v>73</v>
+        <v>61</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" t="s">
-        <v>69</v>
-      </c>
-      <c r="B66" s="8">
-        <v>10.15</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="G66" s="13"/>
-      <c r="H66" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G67" s="13">
-        <v>44436</v>
+        <v>44383</v>
       </c>
       <c r="H67" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>102</v>
+      <c r="B68" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G68" s="13">
-        <v>44436</v>
+        <v>44318</v>
       </c>
       <c r="H68" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="5">
-        <v>12</v>
+      <c r="B69" s="8">
+        <v>10.15</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E69" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="E69" s="5"/>
       <c r="F69" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G69" s="13">
-        <v>44470</v>
-      </c>
+      <c r="G69" s="13"/>
       <c r="H69" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="5">
-        <v>11.4</v>
+      <c r="B70" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>78</v>
       </c>
       <c r="F70" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G70" s="13">
+        <v>44436</v>
+      </c>
+      <c r="H70" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71" s="13">
+        <v>44436</v>
+      </c>
+      <c r="H71" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" t="s">
+        <v>69</v>
+      </c>
+      <c r="B72" s="5">
+        <v>12</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72" s="13">
+        <v>44470</v>
+      </c>
+      <c r="H72" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73" s="5">
+        <v>11.4</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F73" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G70" s="13">
+      <c r="G73" s="13">
         <v>44383</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H73" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
-      <c r="B71" s="5"/>
+    <row r="74" spans="1:8">
+      <c r="B74" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Update test matrix for CentOS 9 and Fedora 37
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="118">
   <si>
     <t>CentOS</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>gcc 12.2.0</t>
+  </si>
+  <si>
+    <t>Stream 9</t>
+  </si>
+  <si>
+    <t>gcc 11.3.1</t>
   </si>
 </sst>
 </file>
@@ -755,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H74"/>
+  <dimension ref="A2:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -784,7 +790,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44855</v>
+        <v>44881</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -906,20 +912,22 @@
         <v>0</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E16" s="5" t="s">
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="13">
-        <v>44210</v>
+        <v>44881</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -927,14 +935,14 @@
         <v>0</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>9</v>
@@ -948,14 +956,14 @@
         <v>0</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>9</v>
@@ -966,49 +974,63 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="13">
+        <v>44210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="5">
-        <v>36</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="B20" s="5">
+        <v>37</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="13">
-        <v>44817</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="13"/>
+      <c r="F20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="13">
+        <v>44880</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="8">
-        <v>11</v>
+        <v>80</v>
+      </c>
+      <c r="B21" s="5">
+        <v>36</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>9</v>
@@ -1018,43 +1040,27 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="13">
-        <v>44817</v>
-      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="5">
-        <v>10.6</v>
+      <c r="B23" s="8">
+        <v>11</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>9</v>
@@ -1067,26 +1073,23 @@
       <c r="A24" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="5">
-        <v>10.6</v>
+      <c r="B24" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G24" s="13">
         <v>44817</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1094,20 +1097,22 @@
         <v>1</v>
       </c>
       <c r="B25" s="5">
-        <v>9.9</v>
+        <v>10.6</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E25" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="13">
-        <v>44177</v>
+        <v>44817</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1115,29 +1120,33 @@
         <v>1</v>
       </c>
       <c r="B26" s="5">
-        <v>8.6</v>
+        <v>10.6</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="5"/>
+      <c r="D26" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E26" s="5" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G26" s="13">
-        <v>44183</v>
-      </c>
-      <c r="H26" s="9"/>
+        <v>44817</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>1</v>
       </c>
       <c r="B27" s="5">
-        <v>8.6</v>
+        <v>9.9</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>86</v>
@@ -1150,9 +1159,8 @@
         <v>9</v>
       </c>
       <c r="G27" s="13">
-        <v>44182</v>
-      </c>
-      <c r="H27" s="9"/>
+        <v>44177</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
@@ -1166,17 +1174,15 @@
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G28" s="13">
-        <v>44185</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>44183</v>
+      </c>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
@@ -1190,17 +1196,15 @@
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G29" s="13">
-        <v>44177</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>44182</v>
+      </c>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
@@ -1214,101 +1218,104 @@
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="13">
+        <v>44185</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5">
+        <v>8.6</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="13">
         <v>44177</v>
       </c>
-      <c r="H30" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="9"/>
+      <c r="H31" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="B32" s="5">
-        <v>15.3</v>
+        <v>8.6</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D32" s="5"/>
       <c r="E32" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G32" s="13">
-        <v>44378</v>
+        <v>44177</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="5">
-        <v>20.04</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="13">
-        <v>44411</v>
-      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="13"/>
       <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="14">
-        <v>22.1</v>
+        <v>88</v>
+      </c>
+      <c r="B34" s="5">
+        <v>15.3</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G34" s="13">
-        <v>44855</v>
+        <v>44378</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B35" s="5">
         <v>20.04</v>
@@ -1321,31 +1328,34 @@
         <v>26</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G35" s="13">
-        <v>44178</v>
-      </c>
+        <v>44411</v>
+      </c>
+      <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="5">
-        <v>18.04</v>
+      <c r="B36" s="14">
+        <v>22.1</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="5"/>
+      <c r="D36" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E36" s="5" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G36" s="13">
-        <v>44177</v>
+        <v>44855</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1353,23 +1363,20 @@
         <v>6</v>
       </c>
       <c r="B37" s="5">
-        <v>16.04</v>
+        <v>20.04</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="G37" s="13">
-        <v>44245</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>54</v>
+        <v>44178</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1377,44 +1384,45 @@
         <v>6</v>
       </c>
       <c r="B38" s="5">
-        <v>12.04</v>
+        <v>18.04</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G38" s="13">
-        <v>44183</v>
-      </c>
-      <c r="H38" s="9"/>
+        <v>44177</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>6</v>
       </c>
       <c r="B39" s="5">
-        <v>12.04</v>
+        <v>16.04</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="G39" s="13">
-        <v>44182</v>
-      </c>
-      <c r="H39" s="9"/>
+        <v>44245</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
@@ -1428,17 +1436,15 @@
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G40" s="13">
-        <v>44177</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>44183</v>
+      </c>
+      <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
@@ -1452,103 +1458,107 @@
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G41" s="13">
+        <v>44182</v>
+      </c>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="5">
+        <v>12.04</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="13">
         <v>44177</v>
       </c>
-      <c r="H41" s="9" t="s">
+      <c r="H42" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="13"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B43" s="5">
-        <v>5.21</v>
+        <v>12.04</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G43" s="13">
-        <v>44383</v>
+        <v>44177</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" s="5">
-        <v>20.04</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G44" s="13">
-        <v>44205</v>
-      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="13"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>10</v>
       </c>
       <c r="B45" s="5">
-        <v>11.19</v>
+        <v>5.21</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="5"/>
+      <c r="D45" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E45" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G45" s="13">
-        <v>44177</v>
+        <v>44383</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B46" s="5">
-        <v>20</v>
+        <v>20.04</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="5"/>
+      <c r="D46" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="E46" s="5" t="s">
         <v>26</v>
       </c>
@@ -1556,104 +1566,106 @@
         <v>9</v>
       </c>
       <c r="G46" s="13">
-        <v>44178</v>
+        <v>44205</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>99</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>100</v>
+        <v>10</v>
+      </c>
+      <c r="B47" s="5">
+        <v>11.19</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="D47" s="5"/>
       <c r="E47" s="5" t="s">
-        <v>101</v>
+        <v>24</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G47" s="13">
-        <v>44483</v>
+        <v>44177</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>87</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>103</v>
+        <v>8</v>
+      </c>
+      <c r="B48" s="5">
+        <v>20</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="5"/>
+      <c r="E48" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G48" s="13">
+        <v>44178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E48" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G48" s="13">
-        <v>44816</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="G49" s="13"/>
+      <c r="E49" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="13">
+        <v>44483</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="5">
-        <v>15.1</v>
+        <v>87</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="5"/>
+      <c r="D50" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="E50" s="5" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G50" s="13">
-        <v>44203</v>
+        <v>44816</v>
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" t="s">
-        <v>48</v>
-      </c>
-      <c r="B51" s="5">
-        <v>15.2</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="G51" s="13"/>
     </row>
-    <row r="52" spans="1:8" ht="15" customHeight="1">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>48</v>
       </c>
       <c r="B52" s="5">
-        <v>15.3</v>
+        <v>15.1</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>5</v>
@@ -1666,148 +1678,142 @@
         <v>9</v>
       </c>
       <c r="G52" s="13">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53" s="5">
+        <v>15.2</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" s="13"/>
+    </row>
+    <row r="54" spans="1:8" ht="15" customHeight="1">
+      <c r="A54" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="5">
+        <v>15.3</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54" s="13">
         <v>44316</v>
       </c>
-      <c r="H52" s="9" t="s">
+      <c r="H54" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="13"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" t="s">
-        <v>11</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G54" s="13">
-        <v>44392</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
     <row r="55" spans="1:8">
-      <c r="A55" t="s">
-        <v>36</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G55" s="13">
-        <v>44817</v>
-      </c>
-      <c r="H55" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>36</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>45</v>
+        <v>11</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G56" s="13">
-        <v>44393</v>
-      </c>
-      <c r="H56" s="9"/>
+        <v>44392</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>6</v>
-      </c>
-      <c r="B57" s="8">
-        <v>21.04</v>
+        <v>36</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>84</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>92</v>
       </c>
       <c r="G57" s="13">
-        <v>44203</v>
+        <v>44817</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G58" s="13">
-        <v>44203</v>
-      </c>
+        <v>44393</v>
+      </c>
+      <c r="H58" s="9"/>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>53</v>
-      </c>
-      <c r="B59" s="5">
-        <v>20.12</v>
+        <v>6</v>
+      </c>
+      <c r="B59" s="8">
+        <v>21.04</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>14</v>
@@ -1816,290 +1822,336 @@
         <v>84</v>
       </c>
       <c r="E59" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G59" s="13">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F59" s="5" t="s">
+      <c r="F60" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G59" s="13">
-        <v>44215</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="G60" s="13"/>
+      <c r="G60" s="13">
+        <v>44203</v>
+      </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>62</v>
-      </c>
-      <c r="B61" s="8">
-        <v>12.2</v>
+        <v>53</v>
+      </c>
+      <c r="B61" s="5">
+        <v>20.12</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>63</v>
+        <v>14</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G61" s="13">
-        <v>44294</v>
-      </c>
-      <c r="H61" s="12" t="s">
-        <v>65</v>
+        <v>44215</v>
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" t="s">
-        <v>62</v>
-      </c>
-      <c r="B62" s="8">
-        <v>12.2</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G62" s="13">
-        <v>44480</v>
-      </c>
-      <c r="H62" s="12"/>
+      <c r="G62" s="13"/>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>66</v>
+      <c r="B63" s="8">
+        <v>12.2</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>63</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G63" s="13">
-        <v>44298</v>
-      </c>
-      <c r="H63" s="12"/>
+        <v>44294</v>
+      </c>
+      <c r="H63" s="12" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>32</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>34</v>
+        <v>62</v>
+      </c>
+      <c r="B64" s="8">
+        <v>12.2</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="F64" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G64" s="13" t="s">
-        <v>35</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="G64" s="13">
+        <v>44480</v>
+      </c>
+      <c r="H64" s="12"/>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>112</v>
-      </c>
-      <c r="B65" s="8">
-        <v>7.1</v>
+        <v>62</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="C65" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G65" s="13">
+        <v>44298</v>
+      </c>
+      <c r="H65" s="12"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" t="s">
+        <v>32</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G65" s="13" t="s">
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G66" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H65" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="G66" s="13"/>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>69</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>71</v>
+        <v>112</v>
+      </c>
+      <c r="B67" s="8">
+        <v>7.1</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="D67" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E67" s="5" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G67" s="13">
-        <v>44383</v>
-      </c>
-      <c r="H67" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="G67" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G68" s="13">
-        <v>44318</v>
-      </c>
-      <c r="H68" t="s">
-        <v>73</v>
-      </c>
+      <c r="G68" s="13"/>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>69</v>
       </c>
-      <c r="B69" s="8">
-        <v>10.15</v>
+      <c r="B69" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E69" s="5"/>
+      <c r="E69" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="F69" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G69" s="13"/>
+      <c r="G69" s="13">
+        <v>44383</v>
+      </c>
       <c r="H69" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>102</v>
+      <c r="B70" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G70" s="13">
-        <v>44436</v>
+        <v>44318</v>
       </c>
       <c r="H70" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>69</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>102</v>
+      <c r="B71" s="8">
+        <v>10.15</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E71" s="5" t="s">
-        <v>78</v>
-      </c>
+      <c r="E71" s="5"/>
       <c r="F71" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G71" s="13">
-        <v>44436</v>
-      </c>
+      <c r="G71" s="13"/>
       <c r="H71" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="5">
-        <v>12</v>
+      <c r="B72" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G72" s="13">
-        <v>44470</v>
+        <v>44436</v>
       </c>
       <c r="H72" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="5">
-        <v>11.4</v>
+      <c r="B73" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>78</v>
       </c>
       <c r="F73" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73" s="13">
+        <v>44436</v>
+      </c>
+      <c r="H73" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" t="s">
+        <v>69</v>
+      </c>
+      <c r="B74" s="5">
+        <v>12</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G74" s="13">
+        <v>44470</v>
+      </c>
+      <c r="H74" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" t="s">
+        <v>69</v>
+      </c>
+      <c r="B75" s="5">
+        <v>11.4</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F75" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G73" s="13">
+      <c r="G75" s="13">
         <v>44383</v>
       </c>
-      <c r="H73" t="s">
+      <c r="H75" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
-      <c r="B74" s="5"/>
+    <row r="76" spans="1:8">
+      <c r="B76" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Update test matrix for Alma and Rocky Linux 9
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="120">
   <si>
     <t>CentOS</t>
   </si>
@@ -370,14 +370,21 @@
   </si>
   <si>
     <t>gcc 11.3.1</t>
+  </si>
+  <si>
+    <t>gcc 11.2.1</t>
+  </si>
+  <si>
+    <t>Rocky</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -428,7 +435,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -464,6 +471,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -761,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H76"/>
+  <dimension ref="A2:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -888,8 +898,8 @@
       <c r="A15" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="5">
-        <v>8.4</v>
+      <c r="B15" s="15">
+        <v>9</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>5</v>
@@ -898,36 +908,36 @@
         <v>50</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="13">
-        <v>44393</v>
+        <v>44881</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>116</v>
+        <v>81</v>
+      </c>
+      <c r="B16" s="5">
+        <v>8.4</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="13">
-        <v>44881</v>
+        <v>44393</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -935,20 +945,22 @@
         <v>0</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E17" s="5" t="s">
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="13">
-        <v>44210</v>
+        <v>44881</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -956,14 +968,14 @@
         <v>0</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>9</v>
@@ -977,14 +989,14 @@
         <v>0</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>9</v>
@@ -995,25 +1007,23 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="5">
-        <v>37</v>
+        <v>0</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>108</v>
+        <v>20</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G20" s="13">
-        <v>44880</v>
+        <v>44210</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1021,13 +1031,13 @@
         <v>80</v>
       </c>
       <c r="B21" s="5">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>108</v>
@@ -1036,77 +1046,77 @@
         <v>9</v>
       </c>
       <c r="G21" s="13">
+        <v>44880</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="5">
+        <v>36</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="13">
         <v>44817</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="13"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="8">
-        <v>11</v>
+        <v>119</v>
+      </c>
+      <c r="B23" s="15">
+        <v>9</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="13">
-        <v>44817</v>
+        <v>44881</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="13">
-        <v>44817</v>
-      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="5">
-        <v>10.6</v>
+      <c r="B25" s="8">
+        <v>11</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>9</v>
@@ -1119,26 +1129,23 @@
       <c r="A26" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="5">
-        <v>10.6</v>
+      <c r="B26" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G26" s="13">
         <v>44817</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1146,20 +1153,22 @@
         <v>1</v>
       </c>
       <c r="B27" s="5">
-        <v>9.9</v>
+        <v>10.6</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E27" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G27" s="13">
-        <v>44177</v>
+        <v>44817</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1167,29 +1176,33 @@
         <v>1</v>
       </c>
       <c r="B28" s="5">
-        <v>8.6</v>
+        <v>10.6</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E28" s="5" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G28" s="13">
-        <v>44183</v>
-      </c>
-      <c r="H28" s="9"/>
+        <v>44817</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="5">
-        <v>8.6</v>
+        <v>9.9</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>86</v>
@@ -1202,9 +1215,8 @@
         <v>9</v>
       </c>
       <c r="G29" s="13">
-        <v>44182</v>
-      </c>
-      <c r="H29" s="9"/>
+        <v>44177</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
@@ -1218,17 +1230,15 @@
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="13">
-        <v>44185</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>44183</v>
+      </c>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
@@ -1242,17 +1252,15 @@
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G31" s="13">
-        <v>44177</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>44182</v>
+      </c>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
@@ -1266,101 +1274,104 @@
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G32" s="13">
+        <v>44185</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="5">
+        <v>8.6</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="13">
         <v>44177</v>
       </c>
-      <c r="H32" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="9"/>
+      <c r="H33" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="B34" s="5">
-        <v>15.3</v>
+        <v>8.6</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G34" s="13">
-        <v>44378</v>
+        <v>44177</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="5">
-        <v>20.04</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="13">
-        <v>44411</v>
-      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="13"/>
       <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="14">
-        <v>22.1</v>
+        <v>88</v>
+      </c>
+      <c r="B36" s="5">
+        <v>15.3</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
       <c r="F36" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G36" s="13">
-        <v>44855</v>
+        <v>44378</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B37" s="5">
         <v>20.04</v>
@@ -1373,31 +1384,34 @@
         <v>26</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G37" s="13">
-        <v>44178</v>
-      </c>
+        <v>44411</v>
+      </c>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="5">
-        <v>18.04</v>
+      <c r="B38" s="14">
+        <v>22.1</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="5"/>
+      <c r="D38" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E38" s="5" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G38" s="13">
-        <v>44177</v>
+        <v>44855</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1405,23 +1419,20 @@
         <v>6</v>
       </c>
       <c r="B39" s="5">
-        <v>16.04</v>
+        <v>20.04</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="G39" s="13">
-        <v>44245</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>54</v>
+        <v>44178</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1429,44 +1440,45 @@
         <v>6</v>
       </c>
       <c r="B40" s="5">
-        <v>12.04</v>
+        <v>18.04</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G40" s="13">
-        <v>44183</v>
-      </c>
-      <c r="H40" s="9"/>
+        <v>44177</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>6</v>
       </c>
       <c r="B41" s="5">
-        <v>12.04</v>
+        <v>16.04</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="G41" s="13">
-        <v>44182</v>
-      </c>
-      <c r="H41" s="9"/>
+        <v>44245</v>
+      </c>
+      <c r="H41" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
@@ -1480,17 +1492,15 @@
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G42" s="13">
-        <v>44177</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>44183</v>
+      </c>
+      <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
@@ -1504,103 +1514,107 @@
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G43" s="13">
+        <v>44182</v>
+      </c>
+      <c r="H43" s="9"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="5">
+        <v>12.04</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="13">
         <v>44177</v>
       </c>
-      <c r="H43" s="9" t="s">
+      <c r="H44" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="13"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B45" s="5">
-        <v>5.21</v>
+        <v>12.04</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G45" s="13">
-        <v>44383</v>
+        <v>44177</v>
+      </c>
+      <c r="H45" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46" s="5">
-        <v>20.04</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46" s="13">
-        <v>44205</v>
-      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="13"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>10</v>
       </c>
       <c r="B47" s="5">
-        <v>11.19</v>
+        <v>5.21</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="5"/>
+      <c r="D47" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E47" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G47" s="13">
-        <v>44177</v>
+        <v>44383</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B48" s="5">
-        <v>20</v>
+        <v>20.04</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="5"/>
+      <c r="D48" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="E48" s="5" t="s">
         <v>26</v>
       </c>
@@ -1608,104 +1622,106 @@
         <v>9</v>
       </c>
       <c r="G48" s="13">
-        <v>44178</v>
+        <v>44205</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>99</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>100</v>
+        <v>10</v>
+      </c>
+      <c r="B49" s="5">
+        <v>11.19</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="D49" s="5"/>
       <c r="E49" s="5" t="s">
-        <v>101</v>
+        <v>24</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G49" s="13">
-        <v>44483</v>
+        <v>44177</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>87</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>103</v>
+        <v>8</v>
+      </c>
+      <c r="B50" s="5">
+        <v>20</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="5"/>
+      <c r="E50" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="13">
+        <v>44178</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E50" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G50" s="13">
-        <v>44816</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="G51" s="13"/>
+      <c r="E51" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" s="13">
+        <v>44483</v>
+      </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>48</v>
-      </c>
-      <c r="B52" s="5">
-        <v>15.1</v>
+        <v>87</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="5"/>
+      <c r="D52" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="E52" s="5" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G52" s="13">
-        <v>44203</v>
+        <v>44816</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" s="5">
-        <v>15.2</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="G53" s="13"/>
     </row>
-    <row r="54" spans="1:8" ht="15" customHeight="1">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>48</v>
       </c>
       <c r="B54" s="5">
-        <v>15.3</v>
+        <v>15.1</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>5</v>
@@ -1718,148 +1734,142 @@
         <v>9</v>
       </c>
       <c r="G54" s="13">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" s="5">
+        <v>15.2</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G55" s="13"/>
+    </row>
+    <row r="56" spans="1:8" ht="15" customHeight="1">
+      <c r="A56" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" s="5">
+        <v>15.3</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" s="13">
         <v>44316</v>
       </c>
-      <c r="H54" s="9" t="s">
+      <c r="H56" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="13"/>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" t="s">
-        <v>11</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G56" s="13">
-        <v>44392</v>
-      </c>
-      <c r="H56" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
     <row r="57" spans="1:8">
-      <c r="A57" t="s">
-        <v>36</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G57" s="13">
-        <v>44817</v>
-      </c>
-      <c r="H57" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>36</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>45</v>
+        <v>11</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>21</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G58" s="13">
-        <v>44393</v>
-      </c>
-      <c r="H58" s="9"/>
+        <v>44392</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>6</v>
-      </c>
-      <c r="B59" s="8">
-        <v>21.04</v>
+        <v>36</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>84</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>92</v>
       </c>
       <c r="G59" s="13">
-        <v>44203</v>
+        <v>44817</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G60" s="13">
-        <v>44203</v>
-      </c>
+        <v>44393</v>
+      </c>
+      <c r="H60" s="9"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>53</v>
-      </c>
-      <c r="B61" s="5">
-        <v>20.12</v>
+        <v>6</v>
+      </c>
+      <c r="B61" s="8">
+        <v>21.04</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>14</v>
@@ -1868,290 +1878,336 @@
         <v>84</v>
       </c>
       <c r="E61" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G61" s="13">
+        <v>44203</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F62" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G61" s="13">
-        <v>44215</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="G62" s="13"/>
+      <c r="G62" s="13">
+        <v>44203</v>
+      </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>62</v>
-      </c>
-      <c r="B63" s="8">
-        <v>12.2</v>
+        <v>53</v>
+      </c>
+      <c r="B63" s="5">
+        <v>20.12</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>63</v>
+        <v>14</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G63" s="13">
-        <v>44294</v>
-      </c>
-      <c r="H63" s="12" t="s">
-        <v>65</v>
+        <v>44215</v>
       </c>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" t="s">
-        <v>62</v>
-      </c>
-      <c r="B64" s="8">
-        <v>12.2</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G64" s="13">
-        <v>44480</v>
-      </c>
-      <c r="H64" s="12"/>
+      <c r="G64" s="13"/>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>62</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>66</v>
+      <c r="B65" s="8">
+        <v>12.2</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>63</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G65" s="13">
-        <v>44298</v>
-      </c>
-      <c r="H65" s="12"/>
+        <v>44294</v>
+      </c>
+      <c r="H65" s="12" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>32</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>34</v>
+        <v>62</v>
+      </c>
+      <c r="B66" s="8">
+        <v>12.2</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="F66" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G66" s="13" t="s">
-        <v>35</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="G66" s="13">
+        <v>44480</v>
+      </c>
+      <c r="H66" s="12"/>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>112</v>
-      </c>
-      <c r="B67" s="8">
-        <v>7.1</v>
+        <v>62</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="C67" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G67" s="13">
+        <v>44298</v>
+      </c>
+      <c r="H67" s="12"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C68" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D67" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G67" s="13" t="s">
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G68" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H67" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
-      <c r="G68" s="13"/>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>69</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>71</v>
+        <v>112</v>
+      </c>
+      <c r="B69" s="8">
+        <v>7.1</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="D69" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="E69" s="5" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G69" s="13">
-        <v>44383</v>
-      </c>
-      <c r="H69" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="G69" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" t="s">
-        <v>69</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G70" s="13">
-        <v>44318</v>
-      </c>
-      <c r="H70" t="s">
-        <v>73</v>
-      </c>
+      <c r="G70" s="13"/>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>69</v>
       </c>
-      <c r="B71" s="8">
-        <v>10.15</v>
+      <c r="B71" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E71" s="5"/>
+      <c r="E71" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="F71" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G71" s="13"/>
+      <c r="G71" s="13">
+        <v>44383</v>
+      </c>
       <c r="H71" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>102</v>
+      <c r="B72" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G72" s="13">
-        <v>44436</v>
+        <v>44318</v>
       </c>
       <c r="H72" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>102</v>
+      <c r="B73" s="8">
+        <v>10.15</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E73" s="5" t="s">
-        <v>78</v>
-      </c>
+      <c r="E73" s="5"/>
       <c r="F73" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G73" s="13">
-        <v>44436</v>
-      </c>
+      <c r="G73" s="13"/>
       <c r="H73" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>69</v>
       </c>
-      <c r="B74" s="5">
-        <v>12</v>
+      <c r="B74" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G74" s="13">
-        <v>44470</v>
+        <v>44436</v>
       </c>
       <c r="H74" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>69</v>
       </c>
-      <c r="B75" s="5">
-        <v>11.4</v>
+      <c r="B75" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>78</v>
       </c>
       <c r="F75" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" s="13">
+        <v>44436</v>
+      </c>
+      <c r="H75" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" t="s">
+        <v>69</v>
+      </c>
+      <c r="B76" s="5">
+        <v>12</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" s="13">
+        <v>44470</v>
+      </c>
+      <c r="H76" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" s="5">
+        <v>11.4</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F77" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G75" s="13">
+      <c r="G77" s="13">
         <v>44383</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
-      <c r="B76" s="5"/>
+    <row r="78" spans="1:8">
+      <c r="B78" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Update README for --accept-root switch
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="121">
   <si>
     <t>CentOS</t>
   </si>
@@ -376,6 +376,9 @@
   </si>
   <si>
     <t>Rocky</t>
+  </si>
+  <si>
+    <t>gcc 11.4.1</t>
   </si>
 </sst>
 </file>
@@ -774,7 +777,7 @@
   <dimension ref="A2:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -800,7 +803,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="4">
         <f ca="1">TODAY()</f>
-        <v>44881</v>
+        <v>45253</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1077,7 +1080,7 @@
         <v>119</v>
       </c>
       <c r="B23" s="15">
-        <v>9</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>5</v>
@@ -1086,13 +1089,13 @@
         <v>50</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="13">
-        <v>44881</v>
+        <v>45253</v>
       </c>
     </row>
     <row r="24" spans="1:8">

</xml_diff>